<commit_message>
rename_with(~ gsub("^x", "", .), starts_with("x"))
</commit_message>
<xml_diff>
--- a/data/milkcowsandprod.xlsx
+++ b/data/milkcowsandprod.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ATeran\AppData\Local\Temp\milkcowsandprod.xlsx_98333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lk/Desktop/p8105/hw_sub/p8105_final_project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EE6731-65AE-40E9-A179-4EDA5CEF1C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F0AE93-EF3B-A94E-9977-859D7B0162F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="773" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="10000" windowHeight="14260" tabRatio="773" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="32" r:id="rId1"/>
@@ -1133,10 +1133,10 @@
     <xf numFmtId="164" fontId="20" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1490,12 +1490,12 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="15.90625" customWidth="1"/>
-    <col min="2" max="2" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1535,7 +1535,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="25.2" customHeight="1">
+    <row r="7" spans="1:2" ht="25.25" customHeight="1">
       <c r="A7" s="86" t="s">
         <v>75</v>
       </c>
@@ -1564,24 +1564,24 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BD83"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AV2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" sqref="A1:B1"/>
+      <selection pane="bottomRight" activeCell="B73" sqref="B73:B74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.81640625" defaultRowHeight="11.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.85546875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="2.54296875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="28.08984375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" style="4" customWidth="1"/>
-    <col min="4" max="55" width="9.81640625" style="4"/>
-    <col min="56" max="56" width="11.36328125" style="4" customWidth="1"/>
-    <col min="57" max="16384" width="9.81640625" style="4"/>
+    <col min="1" max="1" width="2.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="4" customWidth="1"/>
+    <col min="4" max="55" width="9.85546875" style="4"/>
+    <col min="56" max="56" width="11.42578125" style="4" customWidth="1"/>
+    <col min="57" max="16384" width="9.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="28.2" customHeight="1">
+    <row r="1" spans="1:56" ht="28.25" customHeight="1">
       <c r="A1" s="90" t="s">
         <v>82</v>
       </c>
@@ -1637,7 +1637,7 @@
       <c r="AZ1" s="8"/>
       <c r="BA1" s="8"/>
     </row>
-    <row r="2" spans="1:56" ht="18.600000000000001" customHeight="1">
+    <row r="2" spans="1:56" ht="18.5" customHeight="1">
       <c r="A2" s="26"/>
       <c r="B2" s="49" t="s">
         <v>70</v>
@@ -1861,7 +1861,7 @@
       <c r="BB3" s="8"/>
       <c r="BD3" s="25"/>
     </row>
-    <row r="4" spans="1:56" ht="12">
+    <row r="4" spans="1:56">
       <c r="A4" s="39" t="s">
         <v>1</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:56" ht="12">
+    <row r="16" spans="1:56">
       <c r="A16" s="21"/>
       <c r="C16" s="62"/>
       <c r="D16" s="62"/>
@@ -3933,7 +3933,7 @@
       <c r="BC16" s="60"/>
       <c r="BD16" s="61"/>
     </row>
-    <row r="17" spans="1:56" ht="12">
+    <row r="17" spans="1:56">
       <c r="A17" s="39" t="s">
         <v>13</v>
       </c>
@@ -4604,7 +4604,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="21" spans="1:56" ht="12">
+    <row r="21" spans="1:56">
       <c r="A21" s="21"/>
       <c r="C21" s="62"/>
       <c r="D21" s="62"/>
@@ -4661,7 +4661,7 @@
       <c r="BC21" s="60"/>
       <c r="BD21" s="61"/>
     </row>
-    <row r="22" spans="1:56" ht="12">
+    <row r="22" spans="1:56">
       <c r="A22" s="39" t="s">
         <v>17</v>
       </c>
@@ -5668,7 +5668,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:56" ht="12">
+    <row r="28" spans="1:56">
       <c r="A28" s="21"/>
       <c r="C28" s="62"/>
       <c r="D28" s="62"/>
@@ -5725,7 +5725,7 @@
       <c r="BC28" s="60"/>
       <c r="BD28" s="61"/>
     </row>
-    <row r="29" spans="1:56" ht="12">
+    <row r="29" spans="1:56">
       <c r="A29" s="39" t="s">
         <v>23</v>
       </c>
@@ -6564,7 +6564,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="1:56" ht="12">
+    <row r="34" spans="1:56">
       <c r="A34" s="21"/>
       <c r="C34" s="62"/>
       <c r="D34" s="62"/>
@@ -6621,7 +6621,7 @@
       <c r="BC34" s="60"/>
       <c r="BD34" s="61"/>
     </row>
-    <row r="35" spans="1:56" ht="12">
+    <row r="35" spans="1:56">
       <c r="A35" s="39" t="s">
         <v>28</v>
       </c>
@@ -7685,7 +7685,7 @@
       <c r="BC41" s="62"/>
       <c r="BD41" s="63"/>
     </row>
-    <row r="42" spans="1:56" ht="12">
+    <row r="42" spans="1:56">
       <c r="A42" s="39" t="s">
         <v>34</v>
       </c>
@@ -8581,7 +8581,7 @@
       <c r="BC47" s="62"/>
       <c r="BD47" s="63"/>
     </row>
-    <row r="48" spans="1:56" ht="12">
+    <row r="48" spans="1:56">
       <c r="A48" s="39" t="s">
         <v>39</v>
       </c>
@@ -9309,7 +9309,7 @@
       <c r="BC52" s="62"/>
       <c r="BD52" s="63"/>
     </row>
-    <row r="53" spans="1:56" ht="12">
+    <row r="53" spans="1:56">
       <c r="A53" s="39" t="s">
         <v>43</v>
       </c>
@@ -9812,7 +9812,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="56" spans="1:56" ht="12">
+    <row r="56" spans="1:56">
       <c r="A56" s="21"/>
       <c r="C56" s="62"/>
       <c r="D56" s="62"/>
@@ -9869,7 +9869,7 @@
       <c r="BC56" s="60"/>
       <c r="BD56" s="61"/>
     </row>
-    <row r="57" spans="1:56" ht="12">
+    <row r="57" spans="1:56">
       <c r="A57" s="39" t="s">
         <v>80</v>
       </c>
@@ -11437,7 +11437,7 @@
       <c r="BC66" s="62"/>
       <c r="BD66" s="63"/>
     </row>
-    <row r="67" spans="1:56" ht="12">
+    <row r="67" spans="1:56">
       <c r="A67" s="39" t="s">
         <v>61</v>
       </c>
@@ -12108,7 +12108,7 @@
         <v>1714</v>
       </c>
     </row>
-    <row r="71" spans="1:56" ht="12">
+    <row r="71" spans="1:56">
       <c r="A71" s="21"/>
       <c r="C71" s="62"/>
       <c r="D71" s="62"/>
@@ -12668,7 +12668,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="75" spans="1:56" ht="12">
+    <row r="75" spans="1:56">
       <c r="A75" s="21"/>
       <c r="C75" s="62"/>
       <c r="D75" s="62"/>
@@ -12725,7 +12725,7 @@
       <c r="BC75" s="76"/>
       <c r="BD75" s="25"/>
     </row>
-    <row r="76" spans="1:56" ht="12">
+    <row r="76" spans="1:56">
       <c r="A76" s="48" t="s">
         <v>0</v>
       </c>
@@ -12893,7 +12893,7 @@
         <v>9386</v>
       </c>
     </row>
-    <row r="77" spans="1:56" ht="15">
+    <row r="77" spans="1:56" ht="16">
       <c r="A77" s="88" t="s">
         <v>76</v>
       </c>
@@ -12951,7 +12951,7 @@
       <c r="BA77" s="11"/>
       <c r="BB77" s="9"/>
     </row>
-    <row r="78" spans="1:56" ht="43.8" customHeight="1">
+    <row r="78" spans="1:56" ht="43.75" customHeight="1">
       <c r="A78" s="91" t="s">
         <v>77</v>
       </c>
@@ -13009,7 +13009,7 @@
       <c r="BA78" s="11"/>
       <c r="BB78" s="9"/>
     </row>
-    <row r="79" spans="1:56" ht="34.799999999999997" customHeight="1">
+    <row r="79" spans="1:56" ht="34.75" customHeight="1">
       <c r="A79" s="88" t="s">
         <v>78</v>
       </c>
@@ -13062,7 +13062,7 @@
       <c r="AW79" s="7"/>
       <c r="AX79" s="7"/>
     </row>
-    <row r="80" spans="1:56" ht="13.2" customHeight="1">
+    <row r="80" spans="1:56" ht="13.25" customHeight="1">
       <c r="A80" s="6" t="s">
         <v>81</v>
       </c>
@@ -13307,14 +13307,14 @@
       <selection pane="bottomRight" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="3.08984375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="21.6328125" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="8.7265625" style="4"/>
+    <col min="1" max="1" width="3.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" ht="31.2" customHeight="1">
+    <row r="1" spans="1:56" ht="31.25" customHeight="1">
       <c r="A1" s="92" t="s">
         <v>83</v>
       </c>
@@ -13492,7 +13492,7 @@
       <c r="A3" s="21"/>
       <c r="BD3" s="25"/>
     </row>
-    <row r="4" spans="1:56" ht="12">
+    <row r="4" spans="1:56">
       <c r="A4" s="39" t="s">
         <v>1</v>
       </c>
@@ -15507,7 +15507,7 @@
         <v>21150</v>
       </c>
     </row>
-    <row r="16" spans="1:56" ht="12">
+    <row r="16" spans="1:56">
       <c r="A16" s="21"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -15557,7 +15557,7 @@
       <c r="BC16" s="16"/>
       <c r="BD16" s="50"/>
     </row>
-    <row r="17" spans="1:56" ht="12">
+    <row r="17" spans="1:56">
       <c r="A17" s="39" t="s">
         <v>13</v>
       </c>
@@ -16228,7 +16228,7 @@
         <v>23230</v>
       </c>
     </row>
-    <row r="21" spans="1:56" ht="12">
+    <row r="21" spans="1:56">
       <c r="A21" s="21"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -16278,7 +16278,7 @@
       <c r="BC21" s="16"/>
       <c r="BD21" s="50"/>
     </row>
-    <row r="22" spans="1:56" ht="12">
+    <row r="22" spans="1:56">
       <c r="A22" s="39" t="s">
         <v>17</v>
       </c>
@@ -17285,7 +17285,7 @@
         <v>13984</v>
       </c>
     </row>
-    <row r="28" spans="1:56" ht="12">
+    <row r="28" spans="1:56">
       <c r="A28" s="21"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -17335,7 +17335,7 @@
       <c r="BC28" s="16"/>
       <c r="BD28" s="50"/>
     </row>
-    <row r="29" spans="1:56" ht="12">
+    <row r="29" spans="1:56">
       <c r="A29" s="39" t="s">
         <v>23</v>
       </c>
@@ -18174,7 +18174,7 @@
         <v>23733</v>
       </c>
     </row>
-    <row r="34" spans="1:87" ht="12">
+    <row r="34" spans="1:87">
       <c r="A34" s="21"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -18224,7 +18224,7 @@
       <c r="BC34" s="16"/>
       <c r="BD34" s="50"/>
     </row>
-    <row r="35" spans="1:87" ht="12">
+    <row r="35" spans="1:87">
       <c r="A35" s="39" t="s">
         <v>28</v>
       </c>
@@ -19231,7 +19231,7 @@
         <v>18680</v>
       </c>
     </row>
-    <row r="41" spans="1:87" ht="12">
+    <row r="41" spans="1:87">
       <c r="A41" s="21"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
@@ -19281,7 +19281,7 @@
       <c r="BC41" s="16"/>
       <c r="BD41" s="50"/>
     </row>
-    <row r="42" spans="1:87" ht="12">
+    <row r="42" spans="1:87">
       <c r="A42" s="39" t="s">
         <v>34</v>
       </c>
@@ -20150,7 +20150,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="47" spans="1:87" ht="12">
+    <row r="47" spans="1:87">
       <c r="A47" s="21"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
@@ -20200,7 +20200,7 @@
       <c r="BC47" s="16"/>
       <c r="BD47" s="50"/>
     </row>
-    <row r="48" spans="1:87" ht="12">
+    <row r="48" spans="1:87">
       <c r="A48" s="39" t="s">
         <v>39</v>
       </c>
@@ -20871,7 +20871,7 @@
         <v>12625</v>
       </c>
     </row>
-    <row r="52" spans="1:56" ht="12">
+    <row r="52" spans="1:56">
       <c r="A52" s="21"/>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
@@ -20921,7 +20921,7 @@
       <c r="BC52" s="16"/>
       <c r="BD52" s="50"/>
     </row>
-    <row r="53" spans="1:56" ht="12">
+    <row r="53" spans="1:56">
       <c r="A53" s="39" t="s">
         <v>43</v>
       </c>
@@ -21424,7 +21424,7 @@
         <v>25802</v>
       </c>
     </row>
-    <row r="56" spans="1:56" ht="12">
+    <row r="56" spans="1:56">
       <c r="A56" s="21"/>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
@@ -21474,7 +21474,7 @@
       <c r="BC56" s="16"/>
       <c r="BD56" s="50"/>
     </row>
-    <row r="57" spans="1:56" ht="12">
+    <row r="57" spans="1:56">
       <c r="A57" s="39" t="s">
         <v>80</v>
       </c>
@@ -22985,7 +22985,7 @@
         <v>23333</v>
       </c>
     </row>
-    <row r="66" spans="1:56" ht="12">
+    <row r="66" spans="1:56">
       <c r="A66" s="21"/>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
@@ -23035,7 +23035,7 @@
       <c r="BC66" s="16"/>
       <c r="BD66" s="50"/>
     </row>
-    <row r="67" spans="1:56" ht="12">
+    <row r="67" spans="1:56">
       <c r="A67" s="39" t="s">
         <v>61</v>
       </c>
@@ -23706,7 +23706,7 @@
         <v>23863</v>
       </c>
     </row>
-    <row r="71" spans="1:56" ht="12">
+    <row r="71" spans="1:56">
       <c r="A71" s="21"/>
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
@@ -23763,7 +23763,7 @@
       <c r="BC71" s="16"/>
       <c r="BD71" s="50"/>
     </row>
-    <row r="72" spans="1:56" ht="12">
+    <row r="72" spans="1:56">
       <c r="A72" s="39" t="s">
         <v>62</v>
       </c>
@@ -24266,7 +24266,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="75" spans="1:56" ht="12">
+    <row r="75" spans="1:56">
       <c r="A75" s="21"/>
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
@@ -24311,7 +24311,7 @@
       <c r="BC75" s="16"/>
       <c r="BD75" s="50"/>
     </row>
-    <row r="76" spans="1:56" ht="12">
+    <row r="76" spans="1:56">
       <c r="A76" s="48" t="s">
         <v>0</v>
       </c>
@@ -24479,7 +24479,7 @@
         <v>24117</v>
       </c>
     </row>
-    <row r="77" spans="1:56" ht="15">
+    <row r="77" spans="1:56" ht="16">
       <c r="A77" s="88" t="s">
         <v>76</v>
       </c>
@@ -24537,7 +24537,7 @@
       <c r="BA77" s="57"/>
       <c r="BB77" s="16"/>
     </row>
-    <row r="78" spans="1:56" ht="59.4" customHeight="1">
+    <row r="78" spans="1:56" ht="59.5" customHeight="1">
       <c r="A78" s="91" t="s">
         <v>77</v>
       </c>
@@ -24595,7 +24595,7 @@
       <c r="BA78" s="57"/>
       <c r="BB78" s="16"/>
     </row>
-    <row r="79" spans="1:56" ht="40.200000000000003" customHeight="1">
+    <row r="79" spans="1:56" ht="40.25" customHeight="1">
       <c r="A79" s="88" t="s">
         <v>78</v>
       </c>
@@ -24689,118 +24689,118 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="11.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="4.6328125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="26.6328125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="7.81640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6328125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6328125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6328125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6328125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.6328125" style="4" customWidth="1"/>
-    <col min="14" max="14" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.6328125" style="4" customWidth="1"/>
-    <col min="16" max="16" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.6328125" style="4" customWidth="1"/>
-    <col min="18" max="18" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.6328125" style="4" customWidth="1"/>
-    <col min="20" max="20" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.6328125" style="4" customWidth="1"/>
-    <col min="22" max="22" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.6328125" style="4" customWidth="1"/>
-    <col min="24" max="24" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.6328125" style="4" customWidth="1"/>
-    <col min="26" max="26" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.6328125" style="4" customWidth="1"/>
-    <col min="28" max="28" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.6328125" style="4" customWidth="1"/>
-    <col min="30" max="30" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.6328125" style="4" customWidth="1"/>
-    <col min="32" max="32" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.6328125" style="4" customWidth="1"/>
-    <col min="34" max="34" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.6328125" style="4" customWidth="1"/>
-    <col min="36" max="36" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="8.6328125" style="4" customWidth="1"/>
-    <col min="38" max="38" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.6328125" style="4" customWidth="1"/>
-    <col min="40" max="40" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.6328125" style="4" customWidth="1"/>
-    <col min="42" max="42" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.6328125" style="4" customWidth="1"/>
-    <col min="44" max="44" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="8.6328125" style="4" customWidth="1"/>
-    <col min="46" max="46" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="8.6328125" style="4" customWidth="1"/>
-    <col min="48" max="48" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="8.6328125" style="4" customWidth="1"/>
-    <col min="50" max="50" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="8.6328125" style="4" customWidth="1"/>
-    <col min="52" max="52" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.6328125" style="4" customWidth="1"/>
-    <col min="54" max="54" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="8.6328125" style="4" customWidth="1"/>
-    <col min="56" max="56" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="8.6328125" style="4" customWidth="1"/>
-    <col min="58" max="58" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="8.6328125" style="4" customWidth="1"/>
-    <col min="60" max="60" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="8.6328125" style="4" customWidth="1"/>
-    <col min="62" max="62" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="8.6328125" style="4" customWidth="1"/>
-    <col min="64" max="64" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.6328125" style="4" customWidth="1"/>
-    <col min="66" max="66" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="8.6328125" style="4" customWidth="1"/>
-    <col min="68" max="68" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="8.6328125" style="4" customWidth="1"/>
-    <col min="70" max="70" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.6328125" style="4" customWidth="1"/>
-    <col min="72" max="72" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.6328125" style="4" customWidth="1"/>
-    <col min="74" max="74" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="8.6328125" style="4" customWidth="1"/>
-    <col min="76" max="76" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="8.6328125" style="4" customWidth="1"/>
-    <col min="78" max="78" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="8.6328125" style="4" customWidth="1"/>
-    <col min="80" max="80" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="8.6328125" style="4" customWidth="1"/>
-    <col min="82" max="82" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="8.6328125" style="4" customWidth="1"/>
-    <col min="84" max="84" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="8.6328125" style="4" customWidth="1"/>
-    <col min="86" max="86" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="8.6328125" style="4" customWidth="1"/>
-    <col min="88" max="88" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="8.6328125" style="4" customWidth="1"/>
-    <col min="90" max="90" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="8.6328125" style="4" customWidth="1"/>
-    <col min="92" max="92" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="8.6328125" style="4" customWidth="1" collapsed="1"/>
-    <col min="94" max="94" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="8.6328125" style="4" customWidth="1"/>
-    <col min="96" max="96" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="8.6328125" style="4" customWidth="1"/>
-    <col min="98" max="98" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="8.6328125" style="4" customWidth="1"/>
-    <col min="100" max="100" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="8.6328125" style="4" customWidth="1"/>
-    <col min="102" max="102" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="9.1796875" style="4"/>
-    <col min="104" max="104" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="9.1796875" style="4"/>
-    <col min="106" max="106" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="9.1796875" style="4"/>
-    <col min="108" max="108" width="9.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="109" max="110" width="9.6328125" style="4" customWidth="1"/>
-    <col min="111" max="16384" width="9.1796875" style="4"/>
+    <col min="1" max="1" width="4.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="4" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.5703125" style="4" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.5703125" style="4" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.5703125" style="4" customWidth="1"/>
+    <col min="22" max="22" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.5703125" style="4" customWidth="1"/>
+    <col min="24" max="24" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.5703125" style="4" customWidth="1"/>
+    <col min="26" max="26" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.5703125" style="4" customWidth="1"/>
+    <col min="28" max="28" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.5703125" style="4" customWidth="1"/>
+    <col min="30" max="30" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.5703125" style="4" customWidth="1"/>
+    <col min="32" max="32" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.5703125" style="4" customWidth="1"/>
+    <col min="34" max="34" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.5703125" style="4" customWidth="1"/>
+    <col min="36" max="36" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.5703125" style="4" customWidth="1"/>
+    <col min="38" max="38" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.5703125" style="4" customWidth="1"/>
+    <col min="40" max="40" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.5703125" style="4" customWidth="1"/>
+    <col min="42" max="42" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.5703125" style="4" customWidth="1"/>
+    <col min="44" max="44" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="8.5703125" style="4" customWidth="1"/>
+    <col min="46" max="46" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8.5703125" style="4" customWidth="1"/>
+    <col min="48" max="48" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="8.5703125" style="4" customWidth="1"/>
+    <col min="50" max="50" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="8.5703125" style="4" customWidth="1"/>
+    <col min="52" max="52" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="8.5703125" style="4" customWidth="1"/>
+    <col min="54" max="54" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="8.5703125" style="4" customWidth="1"/>
+    <col min="56" max="56" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="8.5703125" style="4" customWidth="1"/>
+    <col min="58" max="58" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="8.5703125" style="4" customWidth="1"/>
+    <col min="60" max="60" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="8.5703125" style="4" customWidth="1"/>
+    <col min="62" max="62" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="8.5703125" style="4" customWidth="1"/>
+    <col min="64" max="64" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.5703125" style="4" customWidth="1"/>
+    <col min="66" max="66" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="8.5703125" style="4" customWidth="1"/>
+    <col min="68" max="68" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="8.5703125" style="4" customWidth="1"/>
+    <col min="70" max="70" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="8.5703125" style="4" customWidth="1"/>
+    <col min="72" max="72" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.5703125" style="4" customWidth="1"/>
+    <col min="74" max="74" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="8.5703125" style="4" customWidth="1"/>
+    <col min="76" max="76" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="8.5703125" style="4" customWidth="1"/>
+    <col min="78" max="78" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="8.5703125" style="4" customWidth="1"/>
+    <col min="80" max="80" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="8.5703125" style="4" customWidth="1"/>
+    <col min="82" max="82" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="8.5703125" style="4" customWidth="1"/>
+    <col min="84" max="84" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="8.5703125" style="4" customWidth="1"/>
+    <col min="86" max="86" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="8.5703125" style="4" customWidth="1"/>
+    <col min="88" max="88" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="8.5703125" style="4" customWidth="1"/>
+    <col min="90" max="90" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="8.5703125" style="4" customWidth="1"/>
+    <col min="92" max="92" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="8.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="94" max="94" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="8.5703125" style="4" customWidth="1"/>
+    <col min="96" max="96" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="8.5703125" style="4" customWidth="1"/>
+    <col min="98" max="98" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="8.5703125" style="4" customWidth="1"/>
+    <col min="100" max="100" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="8.5703125" style="4" customWidth="1"/>
+    <col min="102" max="102" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="9.140625" style="4"/>
+    <col min="104" max="104" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="9.140625" style="4"/>
+    <col min="106" max="106" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="9.140625" style="4"/>
+    <col min="108" max="108" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="109" max="110" width="9.5703125" style="4" customWidth="1"/>
+    <col min="111" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:110" ht="15" customHeight="1">
@@ -24811,12 +24811,12 @@
       <c r="C1" s="2"/>
       <c r="AK1" s="20"/>
       <c r="AL1" s="20"/>
-      <c r="CY1" s="96"/>
-      <c r="CZ1" s="96"/>
-      <c r="DA1" s="96"/>
-      <c r="DB1" s="96"/>
-      <c r="DC1" s="96"/>
-      <c r="DD1" s="96"/>
+      <c r="CY1" s="97"/>
+      <c r="CZ1" s="97"/>
+      <c r="DA1" s="97"/>
+      <c r="DB1" s="97"/>
+      <c r="DC1" s="97"/>
+      <c r="DD1" s="97"/>
       <c r="DE1" s="58"/>
       <c r="DF1" s="58"/>
     </row>
@@ -24829,7 +24829,7 @@
         <v>1970</v>
       </c>
       <c r="D2" s="95"/>
-      <c r="E2" s="97">
+      <c r="E2" s="96">
         <v>1971</v>
       </c>
       <c r="F2" s="95"/>
@@ -25042,7 +25042,7 @@
       </c>
       <c r="DF2" s="95"/>
     </row>
-    <row r="3" spans="1:110" ht="24.9" customHeight="1">
+    <row r="3" spans="1:110" ht="25" customHeight="1">
       <c r="A3" s="21"/>
       <c r="C3" s="23" t="s">
         <v>60</v>
@@ -29429,7 +29429,7 @@
         <v>0.37373433938258738</v>
       </c>
     </row>
-    <row r="17" spans="1:110" ht="12">
+    <row r="17" spans="1:110">
       <c r="A17" s="21"/>
       <c r="B17" s="25"/>
       <c r="C17" s="34"/>
@@ -30861,7 +30861,7 @@
         <v>4.6385467653867227</v>
       </c>
     </row>
-    <row r="22" spans="1:110" ht="12">
+    <row r="22" spans="1:110">
       <c r="A22" s="21"/>
       <c r="B22" s="25"/>
       <c r="C22" s="34"/>
@@ -32953,7 +32953,7 @@
         <v>0.38301143291336076</v>
       </c>
     </row>
-    <row r="29" spans="1:110" ht="12">
+    <row r="29" spans="1:110">
       <c r="A29" s="21"/>
       <c r="B29" s="25"/>
       <c r="C29" s="34"/>
@@ -34715,7 +34715,7 @@
         <v>1.8452580799066989</v>
       </c>
     </row>
-    <row r="35" spans="1:110" ht="12">
+    <row r="35" spans="1:110">
       <c r="A35" s="21"/>
       <c r="B35" s="38"/>
       <c r="C35" s="34"/>
@@ -34827,7 +34827,7 @@
       <c r="DE35" s="78"/>
       <c r="DF35" s="80"/>
     </row>
-    <row r="36" spans="1:110" ht="12">
+    <row r="36" spans="1:110">
       <c r="A36" s="28"/>
       <c r="B36" s="29" t="s">
         <v>28</v>
@@ -36807,7 +36807,7 @@
         <v>0.20630488947005707</v>
       </c>
     </row>
-    <row r="42" spans="1:110" ht="12">
+    <row r="42" spans="1:110">
       <c r="A42" s="21"/>
       <c r="B42" s="25"/>
       <c r="C42" s="34"/>
@@ -36919,7 +36919,7 @@
       <c r="DE42" s="78"/>
       <c r="DF42" s="80"/>
     </row>
-    <row r="43" spans="1:110" ht="12">
+    <row r="43" spans="1:110">
       <c r="A43" s="28"/>
       <c r="B43" s="29" t="s">
         <v>34</v>
@@ -38569,7 +38569,7 @@
         <v>1.236945804103126E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:110" ht="12">
+    <row r="48" spans="1:110">
       <c r="A48" s="21"/>
       <c r="B48" s="25"/>
       <c r="C48" s="34"/>
@@ -40001,7 +40001,7 @@
         <v>4.4618402219434188E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:110" ht="12">
+    <row r="53" spans="1:110">
       <c r="A53" s="21"/>
       <c r="B53" s="25"/>
       <c r="C53" s="34"/>
@@ -41103,7 +41103,7 @@
         <v>7.3178597303458144</v>
       </c>
     </row>
-    <row r="57" spans="1:110" ht="12">
+    <row r="57" spans="1:110">
       <c r="A57" s="21"/>
       <c r="B57" s="25"/>
       <c r="C57" s="34"/>
@@ -44185,7 +44185,7 @@
         <v>0.34016009612835962</v>
       </c>
     </row>
-    <row r="67" spans="1:110" ht="12">
+    <row r="67" spans="1:110">
       <c r="A67" s="21"/>
       <c r="B67" s="25"/>
       <c r="C67" s="34"/>
@@ -45617,7 +45617,7 @@
         <v>18.069127599795021</v>
       </c>
     </row>
-    <row r="72" spans="1:110" ht="12">
+    <row r="72" spans="1:110">
       <c r="A72" s="21"/>
       <c r="B72" s="33"/>
       <c r="C72" s="34"/>
@@ -46719,7 +46719,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="76" spans="1:110" ht="12">
+    <row r="76" spans="1:110">
       <c r="A76" s="21"/>
       <c r="B76" s="25"/>
       <c r="C76" s="34"/>
@@ -47161,7 +47161,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="78" spans="1:110" ht="15">
+    <row r="78" spans="1:110" ht="16">
       <c r="A78" s="88" t="s">
         <v>76</v>
       </c>
@@ -47273,7 +47273,7 @@
       <c r="DE78" s="69"/>
       <c r="DF78" s="56"/>
     </row>
-    <row r="79" spans="1:110" ht="45.6" customHeight="1">
+    <row r="79" spans="1:110" ht="45.5" customHeight="1">
       <c r="A79" s="91" t="s">
         <v>77</v>
       </c>
@@ -47385,7 +47385,7 @@
       <c r="DE79" s="32"/>
       <c r="DF79" s="56"/>
     </row>
-    <row r="80" spans="1:110" ht="34.200000000000003" customHeight="1">
+    <row r="80" spans="1:110" ht="34.25" customHeight="1">
       <c r="A80" s="88" t="s">
         <v>78</v>
       </c>
@@ -47460,7 +47460,7 @@
       <c r="E83" s="7"/>
       <c r="F83" s="7"/>
     </row>
-    <row r="84" spans="1:107" ht="12">
+    <row r="84" spans="1:107">
       <c r="C84" s="16"/>
       <c r="D84" s="16"/>
       <c r="E84" s="16"/>
@@ -47490,7 +47490,7 @@
       <c r="E88" s="7"/>
       <c r="F88" s="7"/>
     </row>
-    <row r="89" spans="1:107" ht="12">
+    <row r="89" spans="1:107">
       <c r="C89" s="16"/>
       <c r="D89" s="16"/>
       <c r="E89" s="16"/>
@@ -47532,7 +47532,7 @@
       <c r="E95" s="7"/>
       <c r="F95" s="7"/>
     </row>
-    <row r="96" spans="1:107" ht="12">
+    <row r="96" spans="1:107">
       <c r="C96" s="16"/>
       <c r="D96" s="16"/>
       <c r="E96" s="16"/>
@@ -47568,7 +47568,7 @@
       <c r="E101" s="7"/>
       <c r="F101" s="7"/>
     </row>
-    <row r="102" spans="3:6" ht="12">
+    <row r="102" spans="3:6">
       <c r="C102" s="16"/>
       <c r="D102" s="16"/>
       <c r="E102" s="16"/>
@@ -47610,7 +47610,7 @@
       <c r="E108" s="7"/>
       <c r="F108" s="7"/>
     </row>
-    <row r="109" spans="3:6" ht="12">
+    <row r="109" spans="3:6">
       <c r="C109" s="16"/>
       <c r="D109" s="16"/>
       <c r="E109" s="16"/>
@@ -47634,7 +47634,7 @@
       <c r="E112" s="7"/>
       <c r="F112" s="7"/>
     </row>
-    <row r="113" spans="3:6" ht="12">
+    <row r="113" spans="3:6">
       <c r="C113" s="16"/>
       <c r="D113" s="16"/>
       <c r="E113" s="16"/>
@@ -47694,7 +47694,7 @@
       <c r="E122" s="7"/>
       <c r="F122" s="7"/>
     </row>
-    <row r="123" spans="3:6" ht="12">
+    <row r="123" spans="3:6">
       <c r="C123" s="16"/>
       <c r="D123" s="16"/>
       <c r="E123" s="16"/>
@@ -47734,7 +47734,7 @@
       <c r="C129" s="7"/>
       <c r="D129" s="7"/>
     </row>
-    <row r="130" spans="3:6" ht="12">
+    <row r="130" spans="3:6">
       <c r="C130" s="16"/>
       <c r="D130" s="16"/>
       <c r="E130" s="16"/>
@@ -47742,20 +47742,36 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="AO2:AP2"/>
-    <mergeCell ref="AQ2:AR2"/>
-    <mergeCell ref="AS2:AT2"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="BK2:BL2"/>
+    <mergeCell ref="CQ2:CR2"/>
+    <mergeCell ref="BU2:BV2"/>
+    <mergeCell ref="CO2:CP2"/>
+    <mergeCell ref="CS2:CT2"/>
+    <mergeCell ref="CU2:CV2"/>
+    <mergeCell ref="CW2:CX2"/>
+    <mergeCell ref="CE2:CF2"/>
+    <mergeCell ref="DC1:DD1"/>
+    <mergeCell ref="DC2:DD2"/>
+    <mergeCell ref="DA1:DB1"/>
+    <mergeCell ref="DA2:DB2"/>
+    <mergeCell ref="CY2:CZ2"/>
+    <mergeCell ref="CY1:CZ1"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="BM2:BN2"/>
+    <mergeCell ref="BO2:BP2"/>
+    <mergeCell ref="BQ2:BR2"/>
+    <mergeCell ref="BS2:BT2"/>
+    <mergeCell ref="AW2:AX2"/>
+    <mergeCell ref="AY2:AZ2"/>
+    <mergeCell ref="BA2:BB2"/>
+    <mergeCell ref="BC2:BD2"/>
+    <mergeCell ref="BE2:BF2"/>
+    <mergeCell ref="BG2:BH2"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AM2:AN2"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="BI2:BJ2"/>
     <mergeCell ref="DE2:DF2"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="S2:T2"/>
@@ -47772,36 +47788,20 @@
     <mergeCell ref="CG2:CH2"/>
     <mergeCell ref="AU2:AV2"/>
     <mergeCell ref="CM2:CN2"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="BM2:BN2"/>
-    <mergeCell ref="BO2:BP2"/>
-    <mergeCell ref="BQ2:BR2"/>
-    <mergeCell ref="BS2:BT2"/>
-    <mergeCell ref="AW2:AX2"/>
-    <mergeCell ref="AY2:AZ2"/>
-    <mergeCell ref="BA2:BB2"/>
-    <mergeCell ref="BC2:BD2"/>
-    <mergeCell ref="BE2:BF2"/>
-    <mergeCell ref="BG2:BH2"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="AM2:AN2"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="BI2:BJ2"/>
-    <mergeCell ref="CU2:CV2"/>
-    <mergeCell ref="CW2:CX2"/>
-    <mergeCell ref="CE2:CF2"/>
-    <mergeCell ref="DC1:DD1"/>
-    <mergeCell ref="DC2:DD2"/>
-    <mergeCell ref="DA1:DB1"/>
-    <mergeCell ref="DA2:DB2"/>
-    <mergeCell ref="CY2:CZ2"/>
-    <mergeCell ref="CY1:CZ1"/>
-    <mergeCell ref="BK2:BL2"/>
-    <mergeCell ref="CQ2:CR2"/>
-    <mergeCell ref="BU2:BV2"/>
-    <mergeCell ref="CO2:CP2"/>
-    <mergeCell ref="CS2:CT2"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="AO2:AP2"/>
+    <mergeCell ref="AQ2:AR2"/>
+    <mergeCell ref="AS2:AT2"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" location="Contents!A1" display="Back to content page." xr:uid="{167FAA7D-7589-435D-AF9F-5AB604A21E08}"/>

</xml_diff>